<commit_message>
Reestructured grid search and tables
</commit_message>
<xml_diff>
--- a/codigo organizado/configuraciontest.xlsx
+++ b/codigo organizado/configuraciontest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio\Documents\antonio\prueba python\codigo organizado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6A7617-4021-4A8B-B766-A8D1E1EDB959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2866A8E-02F6-46FB-937B-90D6A0836FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1038" yWindow="1038" windowWidth="17280" windowHeight="9984" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2952" yWindow="876" windowWidth="17280" windowHeight="9984" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>model</t>
   </si>
@@ -28,9 +28,6 @@
     <t>parameters</t>
   </si>
   <si>
-    <t>max_lags</t>
-  </si>
-  <si>
     <t>tree</t>
   </si>
   <si>
@@ -49,9 +46,6 @@
     <t>lgbm</t>
   </si>
   <si>
-    <t>{'max_depth': [2, 100], 'min_samples_split': [1, 100], 'min_samples_leaf': [2, 100]}</t>
-  </si>
-  <si>
     <t>{'max_depth': [2, 100], 'n_estimators': [1, 100], 'min_samples_leaf': [2, 100],'min_samples_split': [2, 100]}</t>
   </si>
   <si>
@@ -68,6 +62,15 @@
   </si>
   <si>
     <t>horizon</t>
+  </si>
+  <si>
+    <t>{'max_depth': [2, 100], 'min_samples_split': [2, 100], 'min_samples_leaf': [2, 100]}</t>
+  </si>
+  <si>
+    <t>lags</t>
+  </si>
+  <si>
+    <t>[0,5,10,15]</t>
   </si>
 </sst>
 </file>
@@ -444,7 +447,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -457,10 +460,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -468,13 +471,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2">
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D2" s="2">
         <v>6</v>
@@ -482,13 +485,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D3" s="2">
         <v>6</v>
@@ -496,13 +499,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D4" s="2">
         <v>6</v>
@@ -510,13 +513,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2">
         <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D5" s="2">
         <v>6</v>
@@ -524,13 +527,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D6" s="2">
         <v>6</v>
@@ -538,13 +541,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="2">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D7" s="2">
         <v>6</v>

</xml_diff>